<commit_message>
database addjustment for 資料庫建立檢表_wireframe對照
</commit_message>
<xml_diff>
--- a/DataBase/資料庫建立檢表.xlsx
+++ b/DataBase/資料庫建立檢表.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1735" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1739" uniqueCount="383">
   <si>
     <t>Table名稱</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1627,10 +1627,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>應該要和單項總額擇一</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>單日租賃金額</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1644,6 +1640,18 @@
   </si>
   <si>
     <t>建立目前被借走設備之預約序號之紀錄?(才可知道還差幾號才輪到我來計算等待人數)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>租賃頁面N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>預約成功N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2170,63 +2178,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2287,7 +2238,64 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2660,14 +2668,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75" t="s">
+      <c r="B1" s="87"/>
+      <c r="C1" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="75"/>
+      <c r="D1" s="87"/>
       <c r="E1" s="12"/>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -2895,8 +2903,8 @@
       <c r="P9" s="19"/>
       <c r="Q9" s="34"/>
       <c r="R9" s="19"/>
-      <c r="S9" s="73"/>
-      <c r="T9" s="73"/>
+      <c r="S9" s="97"/>
+      <c r="T9" s="97"/>
       <c r="U9" s="19"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -3008,12 +3016,12 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
-      <c r="P13" s="67" t="s">
+      <c r="P13" s="91" t="s">
         <v>289</v>
       </c>
-      <c r="Q13" s="68"/>
-      <c r="R13" s="68"/>
-      <c r="S13" s="68"/>
+      <c r="Q13" s="92"/>
+      <c r="R13" s="92"/>
+      <c r="S13" s="92"/>
       <c r="T13" s="47"/>
       <c r="U13" s="47"/>
       <c r="V13" s="48"/>
@@ -3037,10 +3045,10 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
-      <c r="P14" s="69"/>
-      <c r="Q14" s="70"/>
-      <c r="R14" s="70"/>
-      <c r="S14" s="70"/>
+      <c r="P14" s="93"/>
+      <c r="Q14" s="94"/>
+      <c r="R14" s="94"/>
+      <c r="S14" s="94"/>
       <c r="T14" s="40"/>
       <c r="U14" s="40"/>
       <c r="V14" s="49"/>
@@ -3066,10 +3074,10 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
-      <c r="P15" s="69"/>
-      <c r="Q15" s="70"/>
-      <c r="R15" s="70"/>
-      <c r="S15" s="70"/>
+      <c r="P15" s="93"/>
+      <c r="Q15" s="94"/>
+      <c r="R15" s="94"/>
+      <c r="S15" s="94"/>
       <c r="T15" s="13"/>
       <c r="U15" s="13"/>
       <c r="V15" s="49"/>
@@ -3157,20 +3165,20 @@
       <c r="R19" s="51" t="s">
         <v>198</v>
       </c>
-      <c r="S19" s="74"/>
-      <c r="T19" s="74"/>
+      <c r="S19" s="88"/>
+      <c r="T19" s="88"/>
       <c r="U19" s="13"/>
       <c r="V19" s="49"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="75" t="s">
+      <c r="A20" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="75"/>
-      <c r="C20" s="77" t="s">
+      <c r="B20" s="87"/>
+      <c r="C20" s="90" t="s">
         <v>189</v>
       </c>
-      <c r="D20" s="75"/>
+      <c r="D20" s="87"/>
       <c r="E20" s="12"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
@@ -3415,8 +3423,8 @@
       <c r="R26" s="51" t="s">
         <v>198</v>
       </c>
-      <c r="S26" s="74"/>
-      <c r="T26" s="74"/>
+      <c r="S26" s="88"/>
+      <c r="T26" s="88"/>
       <c r="U26" s="13"/>
       <c r="V26" s="49"/>
     </row>
@@ -3644,8 +3652,8 @@
       <c r="R33" s="51" t="s">
         <v>206</v>
       </c>
-      <c r="S33" s="74"/>
-      <c r="T33" s="74"/>
+      <c r="S33" s="88"/>
+      <c r="T33" s="88"/>
       <c r="U33" s="13"/>
       <c r="V33" s="49"/>
     </row>
@@ -3784,21 +3792,21 @@
       <c r="V37" s="49"/>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="P38" s="71" t="s">
+      <c r="P38" s="95" t="s">
         <v>290</v>
       </c>
-      <c r="Q38" s="72"/>
-      <c r="R38" s="72"/>
-      <c r="S38" s="72"/>
+      <c r="Q38" s="96"/>
+      <c r="R38" s="96"/>
+      <c r="S38" s="96"/>
       <c r="T38" s="13"/>
       <c r="U38" s="13"/>
       <c r="V38" s="49"/>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="P39" s="71"/>
-      <c r="Q39" s="72"/>
-      <c r="R39" s="72"/>
-      <c r="S39" s="72"/>
+      <c r="P39" s="95"/>
+      <c r="Q39" s="96"/>
+      <c r="R39" s="96"/>
+      <c r="S39" s="96"/>
       <c r="T39" s="13"/>
       <c r="U39" s="13"/>
       <c r="V39" s="49"/>
@@ -3822,21 +3830,21 @@
       <c r="Q41" s="51" t="s">
         <v>281</v>
       </c>
-      <c r="R41" s="76"/>
-      <c r="S41" s="76"/>
+      <c r="R41" s="89"/>
+      <c r="S41" s="89"/>
       <c r="T41" s="13"/>
       <c r="U41" s="13"/>
       <c r="V41" s="49"/>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A42" s="75" t="s">
+      <c r="A42" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="75"/>
-      <c r="C42" s="75" t="s">
+      <c r="B42" s="87"/>
+      <c r="C42" s="87" t="s">
         <v>136</v>
       </c>
-      <c r="D42" s="75"/>
+      <c r="D42" s="87"/>
       <c r="E42" s="12"/>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
@@ -4172,8 +4180,8 @@
       <c r="Q50" s="51" t="s">
         <v>281</v>
       </c>
-      <c r="R50" s="76"/>
-      <c r="S50" s="76"/>
+      <c r="R50" s="89"/>
+      <c r="S50" s="89"/>
       <c r="T50" s="13"/>
       <c r="U50" s="13"/>
       <c r="V50" s="49"/>
@@ -4500,14 +4508,14 @@
       <c r="V61" s="63"/>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A62" s="75" t="s">
+      <c r="A62" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B62" s="75"/>
-      <c r="C62" s="75" t="s">
+      <c r="B62" s="87"/>
+      <c r="C62" s="87" t="s">
         <v>249</v>
       </c>
-      <c r="D62" s="75"/>
+      <c r="D62" s="87"/>
       <c r="E62" s="12"/>
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
@@ -5054,14 +5062,14 @@
       <c r="T85" s="13"/>
     </row>
     <row r="86" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="75" t="s">
+      <c r="A86" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B86" s="75"/>
-      <c r="C86" s="75" t="s">
+      <c r="B86" s="87"/>
+      <c r="C86" s="87" t="s">
         <v>246</v>
       </c>
-      <c r="D86" s="75"/>
+      <c r="D86" s="87"/>
       <c r="E86" s="12"/>
       <c r="F86" s="9"/>
       <c r="G86" s="9"/>
@@ -5326,14 +5334,14 @@
       <c r="L96" s="2"/>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A100" s="75" t="s">
+      <c r="A100" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B100" s="75"/>
-      <c r="C100" s="75" t="s">
+      <c r="B100" s="87"/>
+      <c r="C100" s="87" t="s">
         <v>247</v>
       </c>
-      <c r="D100" s="75"/>
+      <c r="D100" s="87"/>
       <c r="E100" s="12"/>
       <c r="F100" s="9"/>
       <c r="G100" s="9"/>
@@ -5616,14 +5624,14 @@
       <c r="L111" s="2"/>
     </row>
     <row r="115" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A115" s="75" t="s">
+      <c r="A115" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B115" s="75"/>
-      <c r="C115" s="75" t="s">
+      <c r="B115" s="87"/>
+      <c r="C115" s="87" t="s">
         <v>160</v>
       </c>
-      <c r="D115" s="75"/>
+      <c r="D115" s="87"/>
       <c r="E115" s="12"/>
       <c r="F115" s="9"/>
       <c r="G115" s="9"/>
@@ -5977,14 +5985,14 @@
       <c r="T128" s="19"/>
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A131" s="75" t="s">
+      <c r="A131" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B131" s="75"/>
-      <c r="C131" s="75" t="s">
+      <c r="B131" s="87"/>
+      <c r="C131" s="87" t="s">
         <v>85</v>
       </c>
-      <c r="D131" s="75"/>
+      <c r="D131" s="87"/>
       <c r="E131" s="12"/>
       <c r="F131" s="9"/>
       <c r="G131" s="9"/>
@@ -6231,14 +6239,14 @@
       <c r="P143" s="13"/>
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A144" s="75" t="s">
+      <c r="A144" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B144" s="75"/>
-      <c r="C144" s="75" t="s">
+      <c r="B144" s="87"/>
+      <c r="C144" s="87" t="s">
         <v>166</v>
       </c>
-      <c r="D144" s="75"/>
+      <c r="D144" s="87"/>
       <c r="E144" s="12"/>
       <c r="F144" s="9"/>
       <c r="G144" s="9"/>
@@ -6423,14 +6431,14 @@
       <c r="L151" s="2"/>
     </row>
     <row r="155" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A155" s="75" t="s">
+      <c r="A155" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B155" s="75"/>
-      <c r="C155" s="75" t="s">
+      <c r="B155" s="87"/>
+      <c r="C155" s="87" t="s">
         <v>237</v>
       </c>
-      <c r="D155" s="75"/>
+      <c r="D155" s="87"/>
       <c r="E155" s="24"/>
       <c r="F155" s="9"/>
       <c r="G155" s="9"/>
@@ -6559,14 +6567,14 @@
       <c r="U161"/>
     </row>
     <row r="162" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A162" s="75" t="s">
+      <c r="A162" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B162" s="75"/>
-      <c r="C162" s="75" t="s">
+      <c r="B162" s="87"/>
+      <c r="C162" s="87" t="s">
         <v>245</v>
       </c>
-      <c r="D162" s="75"/>
+      <c r="D162" s="87"/>
       <c r="E162" s="24"/>
       <c r="F162" s="9"/>
       <c r="G162" s="9"/>
@@ -6690,6 +6698,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="P13:S15"/>
+    <mergeCell ref="P38:S39"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="R41:S41"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:D42"/>
     <mergeCell ref="A155:B155"/>
     <mergeCell ref="C155:D155"/>
     <mergeCell ref="A162:B162"/>
@@ -6706,20 +6728,6 @@
     <mergeCell ref="C100:D100"/>
     <mergeCell ref="A131:B131"/>
     <mergeCell ref="C131:D131"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="P13:S15"/>
-    <mergeCell ref="P38:S39"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="S26:T26"/>
-    <mergeCell ref="R41:S41"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6738,275 +6746,283 @@
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="101" t="s">
         <v>301</v>
       </c>
-      <c r="C1" s="78"/>
-      <c r="E1" s="78" t="s">
+      <c r="C1" s="101"/>
+      <c r="E1" s="101" t="s">
         <v>303</v>
       </c>
-      <c r="F1" s="78"/>
-      <c r="H1" s="81" t="s">
+      <c r="F1" s="101"/>
+      <c r="H1" s="100" t="s">
         <v>306</v>
       </c>
-      <c r="I1" s="81"/>
-      <c r="K1" s="81" t="s">
+      <c r="I1" s="100"/>
+      <c r="K1" s="100" t="s">
         <v>307</v>
       </c>
-      <c r="L1" s="81"/>
-      <c r="N1" s="78" t="s">
+      <c r="L1" s="100"/>
+      <c r="N1" s="101" t="s">
         <v>312</v>
       </c>
-      <c r="O1" s="78"/>
+      <c r="O1" s="101"/>
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="98" t="s">
         <v>302</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="E2" s="79" t="s">
+      <c r="C2" s="99"/>
+      <c r="E2" s="98" t="s">
         <v>304</v>
       </c>
-      <c r="F2" s="80"/>
-      <c r="H2" s="79" t="s">
+      <c r="F2" s="99"/>
+      <c r="H2" s="98" t="s">
         <v>316</v>
       </c>
-      <c r="I2" s="80"/>
-      <c r="K2" s="79" t="s">
+      <c r="I2" s="99"/>
+      <c r="K2" s="98" t="s">
         <v>317</v>
       </c>
-      <c r="L2" s="80"/>
-      <c r="N2" s="79" t="s">
+      <c r="L2" s="99"/>
+      <c r="N2" s="98" t="s">
         <v>321</v>
       </c>
-      <c r="O2" s="80"/>
+      <c r="O2" s="99"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="80"/>
-      <c r="N3" s="80"/>
-      <c r="O3" s="80"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="N3" s="99"/>
+      <c r="O3" s="99"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="80"/>
-      <c r="C4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="80"/>
-      <c r="K4" s="80"/>
-      <c r="L4" s="80"/>
-      <c r="N4" s="80"/>
-      <c r="O4" s="80"/>
+      <c r="B4" s="99"/>
+      <c r="C4" s="99"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="99"/>
+      <c r="K4" s="99"/>
+      <c r="L4" s="99"/>
+      <c r="N4" s="99"/>
+      <c r="O4" s="99"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="H5" s="80"/>
-      <c r="I5" s="80"/>
-      <c r="K5" s="80"/>
-      <c r="L5" s="80"/>
-      <c r="N5" s="80"/>
-      <c r="O5" s="80"/>
+      <c r="B5" s="99"/>
+      <c r="C5" s="99"/>
+      <c r="E5" s="99"/>
+      <c r="F5" s="99"/>
+      <c r="H5" s="99"/>
+      <c r="I5" s="99"/>
+      <c r="K5" s="99"/>
+      <c r="L5" s="99"/>
+      <c r="N5" s="99"/>
+      <c r="O5" s="99"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="80"/>
-      <c r="C6" s="80"/>
-      <c r="E6" s="80"/>
-      <c r="F6" s="80"/>
-      <c r="H6" s="80"/>
-      <c r="I6" s="80"/>
-      <c r="K6" s="80"/>
-      <c r="L6" s="80"/>
-      <c r="N6" s="80"/>
-      <c r="O6" s="80"/>
+      <c r="B6" s="99"/>
+      <c r="C6" s="99"/>
+      <c r="E6" s="99"/>
+      <c r="F6" s="99"/>
+      <c r="H6" s="99"/>
+      <c r="I6" s="99"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="99"/>
+      <c r="N6" s="99"/>
+      <c r="O6" s="99"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="H7" s="80"/>
-      <c r="I7" s="80"/>
-      <c r="K7" s="80"/>
-      <c r="L7" s="80"/>
-      <c r="N7" s="80"/>
-      <c r="O7" s="80"/>
+      <c r="B7" s="99"/>
+      <c r="C7" s="99"/>
+      <c r="E7" s="99"/>
+      <c r="F7" s="99"/>
+      <c r="H7" s="99"/>
+      <c r="I7" s="99"/>
+      <c r="K7" s="99"/>
+      <c r="L7" s="99"/>
+      <c r="N7" s="99"/>
+      <c r="O7" s="99"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="80"/>
-      <c r="C8" s="80"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="80"/>
-      <c r="H8" s="80"/>
-      <c r="I8" s="80"/>
-      <c r="K8" s="80"/>
-      <c r="L8" s="80"/>
-      <c r="N8" s="80"/>
-      <c r="O8" s="80"/>
+      <c r="B8" s="99"/>
+      <c r="C8" s="99"/>
+      <c r="E8" s="99"/>
+      <c r="F8" s="99"/>
+      <c r="H8" s="99"/>
+      <c r="I8" s="99"/>
+      <c r="K8" s="99"/>
+      <c r="L8" s="99"/>
+      <c r="N8" s="99"/>
+      <c r="O8" s="99"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="78" t="s">
+      <c r="B11" s="101" t="s">
         <v>310</v>
       </c>
-      <c r="C11" s="78"/>
-      <c r="E11" s="78" t="s">
+      <c r="C11" s="101"/>
+      <c r="E11" s="101" t="s">
         <v>315</v>
       </c>
-      <c r="F11" s="78"/>
-      <c r="H11" s="81" t="s">
+      <c r="F11" s="101"/>
+      <c r="H11" s="100" t="s">
         <v>305</v>
       </c>
-      <c r="I11" s="81"/>
-      <c r="K11" s="81" t="s">
+      <c r="I11" s="100"/>
+      <c r="K11" s="100" t="s">
         <v>308</v>
       </c>
-      <c r="L11" s="81"/>
-      <c r="N11" s="78" t="s">
+      <c r="L11" s="100"/>
+      <c r="N11" s="101" t="s">
         <v>311</v>
       </c>
-      <c r="O11" s="78"/>
+      <c r="O11" s="101"/>
     </row>
     <row r="12" spans="2:15" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="79" t="s">
+      <c r="B12" s="98" t="s">
         <v>319</v>
       </c>
-      <c r="C12" s="80"/>
-      <c r="E12" s="79" t="s">
+      <c r="C12" s="99"/>
+      <c r="E12" s="98" t="s">
         <v>322</v>
       </c>
-      <c r="F12" s="80"/>
-      <c r="H12" s="79" t="s">
+      <c r="F12" s="99"/>
+      <c r="H12" s="98" t="s">
         <v>309</v>
       </c>
-      <c r="I12" s="80"/>
-      <c r="K12" s="79" t="s">
+      <c r="I12" s="99"/>
+      <c r="K12" s="98" t="s">
         <v>318</v>
       </c>
-      <c r="L12" s="80"/>
-      <c r="N12" s="79" t="s">
+      <c r="L12" s="99"/>
+      <c r="N12" s="98" t="s">
         <v>320</v>
       </c>
-      <c r="O12" s="80"/>
+      <c r="O12" s="99"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="80"/>
-      <c r="C13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="H13" s="80"/>
-      <c r="I13" s="80"/>
-      <c r="K13" s="80"/>
-      <c r="L13" s="80"/>
-      <c r="N13" s="80"/>
-      <c r="O13" s="80"/>
+      <c r="B13" s="99"/>
+      <c r="C13" s="99"/>
+      <c r="E13" s="99"/>
+      <c r="F13" s="99"/>
+      <c r="H13" s="99"/>
+      <c r="I13" s="99"/>
+      <c r="K13" s="99"/>
+      <c r="L13" s="99"/>
+      <c r="N13" s="99"/>
+      <c r="O13" s="99"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="H14" s="80"/>
-      <c r="I14" s="80"/>
-      <c r="K14" s="80"/>
-      <c r="L14" s="80"/>
-      <c r="N14" s="80"/>
-      <c r="O14" s="80"/>
+      <c r="B14" s="99"/>
+      <c r="C14" s="99"/>
+      <c r="E14" s="99"/>
+      <c r="F14" s="99"/>
+      <c r="H14" s="99"/>
+      <c r="I14" s="99"/>
+      <c r="K14" s="99"/>
+      <c r="L14" s="99"/>
+      <c r="N14" s="99"/>
+      <c r="O14" s="99"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="80"/>
-      <c r="C15" s="80"/>
-      <c r="E15" s="80"/>
-      <c r="F15" s="80"/>
-      <c r="H15" s="80"/>
-      <c r="I15" s="80"/>
-      <c r="K15" s="80"/>
-      <c r="L15" s="80"/>
-      <c r="N15" s="80"/>
-      <c r="O15" s="80"/>
+      <c r="B15" s="99"/>
+      <c r="C15" s="99"/>
+      <c r="E15" s="99"/>
+      <c r="F15" s="99"/>
+      <c r="H15" s="99"/>
+      <c r="I15" s="99"/>
+      <c r="K15" s="99"/>
+      <c r="L15" s="99"/>
+      <c r="N15" s="99"/>
+      <c r="O15" s="99"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="80"/>
-      <c r="C16" s="80"/>
-      <c r="E16" s="80"/>
-      <c r="F16" s="80"/>
-      <c r="H16" s="80"/>
-      <c r="I16" s="80"/>
-      <c r="K16" s="80"/>
-      <c r="L16" s="80"/>
-      <c r="N16" s="80"/>
-      <c r="O16" s="80"/>
+      <c r="B16" s="99"/>
+      <c r="C16" s="99"/>
+      <c r="E16" s="99"/>
+      <c r="F16" s="99"/>
+      <c r="H16" s="99"/>
+      <c r="I16" s="99"/>
+      <c r="K16" s="99"/>
+      <c r="L16" s="99"/>
+      <c r="N16" s="99"/>
+      <c r="O16" s="99"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="80"/>
-      <c r="C17" s="80"/>
-      <c r="E17" s="80"/>
-      <c r="F17" s="80"/>
-      <c r="H17" s="80"/>
-      <c r="I17" s="80"/>
-      <c r="K17" s="80"/>
-      <c r="L17" s="80"/>
-      <c r="N17" s="80"/>
-      <c r="O17" s="80"/>
+      <c r="B17" s="99"/>
+      <c r="C17" s="99"/>
+      <c r="E17" s="99"/>
+      <c r="F17" s="99"/>
+      <c r="H17" s="99"/>
+      <c r="I17" s="99"/>
+      <c r="K17" s="99"/>
+      <c r="L17" s="99"/>
+      <c r="N17" s="99"/>
+      <c r="O17" s="99"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="80"/>
-      <c r="C18" s="80"/>
-      <c r="E18" s="80"/>
-      <c r="F18" s="80"/>
-      <c r="H18" s="80"/>
-      <c r="I18" s="80"/>
-      <c r="K18" s="80"/>
-      <c r="L18" s="80"/>
-      <c r="N18" s="80"/>
-      <c r="O18" s="80"/>
+      <c r="B18" s="99"/>
+      <c r="C18" s="99"/>
+      <c r="E18" s="99"/>
+      <c r="F18" s="99"/>
+      <c r="H18" s="99"/>
+      <c r="I18" s="99"/>
+      <c r="K18" s="99"/>
+      <c r="L18" s="99"/>
+      <c r="N18" s="99"/>
+      <c r="O18" s="99"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E21" s="78" t="s">
+      <c r="E21" s="101" t="s">
         <v>313</v>
       </c>
-      <c r="F21" s="78"/>
+      <c r="F21" s="101"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E22" s="79" t="s">
+      <c r="E22" s="98" t="s">
         <v>314</v>
       </c>
-      <c r="F22" s="80"/>
+      <c r="F22" s="99"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E23" s="80"/>
-      <c r="F23" s="80"/>
+      <c r="E23" s="99"/>
+      <c r="F23" s="99"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E24" s="80"/>
-      <c r="F24" s="80"/>
+      <c r="E24" s="99"/>
+      <c r="F24" s="99"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E25" s="80"/>
-      <c r="F25" s="80"/>
+      <c r="E25" s="99"/>
+      <c r="F25" s="99"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E26" s="80"/>
-      <c r="F26" s="80"/>
+      <c r="E26" s="99"/>
+      <c r="F26" s="99"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E27" s="80"/>
-      <c r="F27" s="80"/>
+      <c r="E27" s="99"/>
+      <c r="F27" s="99"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E28" s="80"/>
-      <c r="F28" s="80"/>
+      <c r="E28" s="99"/>
+      <c r="F28" s="99"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N12:O18"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="N2:O8"/>
+    <mergeCell ref="B2:C8"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C18"/>
     <mergeCell ref="E22:F28"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="K2:L8"/>
@@ -7021,14 +7037,6 @@
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="H12:I18"/>
     <mergeCell ref="E21:F21"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N12:O18"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="N2:O8"/>
-    <mergeCell ref="B2:C8"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7070,14 +7078,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75" t="s">
+      <c r="B1" s="87"/>
+      <c r="C1" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="75"/>
+      <c r="D1" s="87"/>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -7250,14 +7258,14 @@
       <c r="J11" s="2"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="75" t="s">
+      <c r="A16" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="75"/>
-      <c r="C16" s="77" t="s">
+      <c r="B16" s="87"/>
+      <c r="C16" s="90" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="75"/>
+      <c r="D16" s="87"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
@@ -7426,14 +7434,14 @@
       <c r="J25" s="2"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="75" t="s">
+      <c r="A30" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="75"/>
-      <c r="C30" s="75" t="s">
+      <c r="B30" s="87"/>
+      <c r="C30" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="75"/>
+      <c r="D30" s="87"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
@@ -7554,14 +7562,14 @@
       <c r="J36" s="2"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="75" t="s">
+      <c r="A41" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="75"/>
-      <c r="C41" s="75" t="s">
+      <c r="B41" s="87"/>
+      <c r="C41" s="87" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="75"/>
+      <c r="D41" s="87"/>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
@@ -7730,14 +7738,14 @@
       <c r="J50" s="2"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="75" t="s">
+      <c r="A55" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B55" s="75"/>
-      <c r="C55" s="75" t="s">
+      <c r="B55" s="87"/>
+      <c r="C55" s="87" t="s">
         <v>61</v>
       </c>
-      <c r="D55" s="75"/>
+      <c r="D55" s="87"/>
       <c r="E55" s="9"/>
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
@@ -7858,14 +7866,14 @@
       <c r="J61" s="2"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="75" t="s">
+      <c r="A66" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B66" s="75"/>
-      <c r="C66" s="75" t="s">
+      <c r="B66" s="87"/>
+      <c r="C66" s="87" t="s">
         <v>68</v>
       </c>
-      <c r="D66" s="75"/>
+      <c r="D66" s="87"/>
       <c r="E66" s="9"/>
       <c r="F66" s="9"/>
       <c r="G66" s="9"/>
@@ -7986,14 +7994,14 @@
       <c r="J72" s="2"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="75" t="s">
+      <c r="A77" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B77" s="75"/>
-      <c r="C77" s="75" t="s">
+      <c r="B77" s="87"/>
+      <c r="C77" s="87" t="s">
         <v>69</v>
       </c>
-      <c r="D77" s="75"/>
+      <c r="D77" s="87"/>
       <c r="E77" s="9"/>
       <c r="F77" s="9"/>
       <c r="G77" s="9"/>
@@ -8162,14 +8170,14 @@
       <c r="J86" s="2"/>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" s="75" t="s">
+      <c r="A91" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B91" s="75"/>
-      <c r="C91" s="75" t="s">
+      <c r="B91" s="87"/>
+      <c r="C91" s="87" t="s">
         <v>74</v>
       </c>
-      <c r="D91" s="75"/>
+      <c r="D91" s="87"/>
       <c r="E91" s="9"/>
       <c r="F91" s="9"/>
       <c r="G91" s="9"/>
@@ -8354,14 +8362,14 @@
       <c r="J101" s="2"/>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106" s="75" t="s">
+      <c r="A106" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B106" s="75"/>
-      <c r="C106" s="75" t="s">
+      <c r="B106" s="87"/>
+      <c r="C106" s="87" t="s">
         <v>81</v>
       </c>
-      <c r="D106" s="75"/>
+      <c r="D106" s="87"/>
       <c r="E106" s="9"/>
       <c r="F106" s="9"/>
       <c r="G106" s="9"/>
@@ -8434,14 +8442,14 @@
       <c r="J109" s="2"/>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A114" s="75" t="s">
+      <c r="A114" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B114" s="75"/>
-      <c r="C114" s="75" t="s">
+      <c r="B114" s="87"/>
+      <c r="C114" s="87" t="s">
         <v>84</v>
       </c>
-      <c r="D114" s="75"/>
+      <c r="D114" s="87"/>
       <c r="E114" s="9"/>
       <c r="F114" s="9"/>
       <c r="G114" s="9"/>
@@ -8514,14 +8522,14 @@
       <c r="J117" s="2"/>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A122" s="75" t="s">
+      <c r="A122" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B122" s="75"/>
-      <c r="C122" s="75" t="s">
+      <c r="B122" s="87"/>
+      <c r="C122" s="87" t="s">
         <v>85</v>
       </c>
-      <c r="D122" s="75"/>
+      <c r="D122" s="87"/>
       <c r="E122" s="9"/>
       <c r="F122" s="9"/>
       <c r="G122" s="9"/>
@@ -8659,6 +8667,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="C66:D66"/>
     <mergeCell ref="A114:B114"/>
     <mergeCell ref="C114:D114"/>
     <mergeCell ref="A122:B122"/>
@@ -8669,18 +8689,6 @@
     <mergeCell ref="C91:D91"/>
     <mergeCell ref="A106:B106"/>
     <mergeCell ref="C106:D106"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:D30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8696,13 +8704,13 @@
   <dimension ref="A1:AA180"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D135" sqref="D135"/>
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="19.625" customWidth="1"/>
-    <col min="3" max="3" width="19.625" style="90" customWidth="1"/>
+    <col min="3" max="3" width="19.625" style="71" customWidth="1"/>
     <col min="4" max="4" width="19.625" customWidth="1"/>
     <col min="5" max="5" width="34.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5" customWidth="1"/>
@@ -8723,20 +8731,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="75"/>
+      <c r="B1" s="87"/>
       <c r="C1" s="64" t="s">
         <v>323</v>
       </c>
       <c r="D1" s="64" t="s">
         <v>324</v>
       </c>
-      <c r="E1" s="84" t="s">
+      <c r="E1" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="85"/>
+      <c r="F1" s="103"/>
       <c r="G1" s="64"/>
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
@@ -8796,7 +8804,7 @@
       <c r="B3" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="86"/>
+      <c r="C3" s="67"/>
       <c r="D3" s="1"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
@@ -8826,7 +8834,7 @@
       <c r="B4" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="86" t="s">
+      <c r="C4" s="67" t="s">
         <v>326</v>
       </c>
       <c r="D4" s="1"/>
@@ -8859,10 +8867,10 @@
       <c r="B5" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C5" s="86" t="s">
+      <c r="C5" s="67" t="s">
         <v>326</v>
       </c>
-      <c r="D5" s="101" t="s">
+      <c r="D5" s="82" t="s">
         <v>327</v>
       </c>
       <c r="E5" s="2"/>
@@ -8889,7 +8897,7 @@
       <c r="B6" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="86" t="s">
+      <c r="C6" s="67" t="s">
         <v>326</v>
       </c>
       <c r="D6" s="1"/>
@@ -8917,7 +8925,7 @@
       <c r="B7" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C7" s="86" t="s">
+      <c r="C7" s="67" t="s">
         <v>325</v>
       </c>
       <c r="D7" s="1"/>
@@ -8945,7 +8953,7 @@
       <c r="B8" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C8" s="86" t="s">
+      <c r="C8" s="67" t="s">
         <v>326</v>
       </c>
       <c r="D8" s="1"/>
@@ -8973,7 +8981,7 @@
       <c r="B9" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C9" s="86" t="s">
+      <c r="C9" s="67" t="s">
         <v>326</v>
       </c>
       <c r="D9" s="1"/>
@@ -8994,8 +9002,8 @@
       <c r="R9" s="19"/>
       <c r="S9" s="34"/>
       <c r="T9" s="19"/>
-      <c r="U9" s="73"/>
-      <c r="V9" s="73"/>
+      <c r="U9" s="97"/>
+      <c r="V9" s="97"/>
       <c r="W9" s="19"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -9005,7 +9013,7 @@
       <c r="B10" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="86" t="s">
+      <c r="C10" s="67" t="s">
         <v>326</v>
       </c>
       <c r="D10" s="1"/>
@@ -9039,10 +9047,10 @@
       <c r="B11" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C11" s="86" t="s">
+      <c r="C11" s="67" t="s">
         <v>325</v>
       </c>
-      <c r="D11" s="101" t="s">
+      <c r="D11" s="82" t="s">
         <v>328</v>
       </c>
       <c r="E11" s="2"/>
@@ -9075,7 +9083,7 @@
       <c r="B12" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C12" s="86" t="s">
+      <c r="C12" s="67" t="s">
         <v>325</v>
       </c>
       <c r="D12" s="1"/>
@@ -9107,7 +9115,7 @@
       <c r="B13" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C13" s="86" t="s">
+      <c r="C13" s="67" t="s">
         <v>325</v>
       </c>
       <c r="D13" s="1"/>
@@ -9125,12 +9133,12 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
-      <c r="R13" s="67" t="s">
+      <c r="R13" s="91" t="s">
         <v>289</v>
       </c>
-      <c r="S13" s="68"/>
-      <c r="T13" s="68"/>
-      <c r="U13" s="68"/>
+      <c r="S13" s="92"/>
+      <c r="T13" s="92"/>
+      <c r="U13" s="92"/>
       <c r="V13" s="47"/>
       <c r="W13" s="47"/>
       <c r="X13" s="48"/>
@@ -9142,7 +9150,7 @@
       <c r="B14" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="C14" s="87" t="s">
+      <c r="C14" s="68" t="s">
         <v>329</v>
       </c>
       <c r="D14" s="6"/>
@@ -9158,10 +9166,10 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
-      <c r="R14" s="69"/>
-      <c r="S14" s="70"/>
-      <c r="T14" s="70"/>
-      <c r="U14" s="70"/>
+      <c r="R14" s="93"/>
+      <c r="S14" s="94"/>
+      <c r="T14" s="94"/>
+      <c r="U14" s="94"/>
       <c r="V14" s="40"/>
       <c r="W14" s="40"/>
       <c r="X14" s="49"/>
@@ -9173,7 +9181,7 @@
       <c r="B15" s="46" t="s">
         <v>296</v>
       </c>
-      <c r="C15" s="88" t="s">
+      <c r="C15" s="69" t="s">
         <v>326</v>
       </c>
       <c r="D15" s="46"/>
@@ -9191,10 +9199,10 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
-      <c r="R15" s="69"/>
-      <c r="S15" s="70"/>
-      <c r="T15" s="70"/>
-      <c r="U15" s="70"/>
+      <c r="R15" s="93"/>
+      <c r="S15" s="94"/>
+      <c r="T15" s="94"/>
+      <c r="U15" s="94"/>
       <c r="V15" s="13"/>
       <c r="W15" s="13"/>
       <c r="X15" s="49"/>
@@ -9206,7 +9214,7 @@
       <c r="B16" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="C16" s="87" t="s">
+      <c r="C16" s="68" t="s">
         <v>325</v>
       </c>
       <c r="D16" s="6"/>
@@ -9237,7 +9245,7 @@
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
       <c r="B17" s="29"/>
-      <c r="C17" s="89"/>
+      <c r="C17" s="70"/>
       <c r="D17" s="29"/>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
@@ -9260,7 +9268,7 @@
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="29"/>
       <c r="B18" s="29"/>
-      <c r="C18" s="89"/>
+      <c r="C18" s="70"/>
       <c r="D18" s="29"/>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
@@ -9290,26 +9298,26 @@
       <c r="T19" s="51" t="s">
         <v>198</v>
       </c>
-      <c r="U19" s="74"/>
-      <c r="V19" s="74"/>
+      <c r="U19" s="88"/>
+      <c r="V19" s="88"/>
       <c r="W19" s="13"/>
       <c r="X19" s="49"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A20" s="75" t="s">
+      <c r="A20" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="75"/>
+      <c r="B20" s="87"/>
       <c r="C20" s="64" t="s">
         <v>323</v>
       </c>
       <c r="D20" s="64" t="s">
         <v>324</v>
       </c>
-      <c r="E20" s="82" t="s">
+      <c r="E20" s="102" t="s">
         <v>189</v>
       </c>
-      <c r="F20" s="83"/>
+      <c r="F20" s="106"/>
       <c r="G20" s="64"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
@@ -9393,7 +9401,7 @@
       <c r="B22" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="C22" s="91"/>
+      <c r="C22" s="72"/>
       <c r="D22" s="31"/>
       <c r="E22" s="31" t="s">
         <v>255</v>
@@ -9433,7 +9441,7 @@
       <c r="B23" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C23" s="86" t="s">
+      <c r="C23" s="67" t="s">
         <v>326</v>
       </c>
       <c r="D23" s="1"/>
@@ -9477,7 +9485,7 @@
       <c r="B24" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C24" s="86" t="s">
+      <c r="C24" s="67" t="s">
         <v>326</v>
       </c>
       <c r="D24" s="1"/>
@@ -9508,10 +9516,10 @@
       <c r="B25" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="86" t="s">
+      <c r="C25" s="67" t="s">
         <v>326</v>
       </c>
-      <c r="D25" s="101" t="s">
+      <c r="D25" s="82" t="s">
         <v>333</v>
       </c>
       <c r="E25" s="17" t="s">
@@ -9549,10 +9557,10 @@
       <c r="B26" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C26" s="86" t="s">
+      <c r="C26" s="67" t="s">
         <v>326</v>
       </c>
-      <c r="D26" s="101"/>
+      <c r="D26" s="82"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2" t="s">
         <v>177</v>
@@ -9576,8 +9584,8 @@
       <c r="T26" s="51" t="s">
         <v>198</v>
       </c>
-      <c r="U26" s="74"/>
-      <c r="V26" s="74"/>
+      <c r="U26" s="88"/>
+      <c r="V26" s="88"/>
       <c r="W26" s="13"/>
       <c r="X26" s="49"/>
     </row>
@@ -9588,10 +9596,10 @@
       <c r="B27" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C27" s="86" t="s">
+      <c r="C27" s="67" t="s">
         <v>326</v>
       </c>
-      <c r="D27" s="101" t="s">
+      <c r="D27" s="82" t="s">
         <v>330</v>
       </c>
       <c r="E27" s="2"/>
@@ -9629,10 +9637,10 @@
       <c r="B28" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C28" s="86" t="s">
+      <c r="C28" s="67" t="s">
         <v>334</v>
       </c>
-      <c r="D28" s="101" t="s">
+      <c r="D28" s="82" t="s">
         <v>330</v>
       </c>
       <c r="E28" s="2"/>
@@ -9668,10 +9676,10 @@
       <c r="B29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="86" t="s">
+      <c r="C29" s="67" t="s">
         <v>326</v>
       </c>
-      <c r="D29" s="101" t="s">
+      <c r="D29" s="82" t="s">
         <v>330</v>
       </c>
       <c r="E29" s="2"/>
@@ -9707,10 +9715,10 @@
       <c r="B30" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="86" t="s">
+      <c r="C30" s="67" t="s">
         <v>326</v>
       </c>
-      <c r="D30" s="101" t="s">
+      <c r="D30" s="82" t="s">
         <v>330</v>
       </c>
       <c r="E30" s="2"/>
@@ -9742,7 +9750,7 @@
       <c r="B31" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="C31" s="87" t="s">
+      <c r="C31" s="68" t="s">
         <v>332</v>
       </c>
       <c r="D31" s="6"/>
@@ -9775,7 +9783,7 @@
       <c r="B32" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C32" s="87" t="s">
+      <c r="C32" s="68" t="s">
         <v>335</v>
       </c>
       <c r="D32" s="6"/>
@@ -9812,7 +9820,7 @@
       <c r="B33" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="C33" s="87" t="s">
+      <c r="C33" s="68" t="s">
         <v>326</v>
       </c>
       <c r="D33" s="6"/>
@@ -9841,8 +9849,8 @@
       <c r="T33" s="51" t="s">
         <v>206</v>
       </c>
-      <c r="U33" s="74"/>
-      <c r="V33" s="74"/>
+      <c r="U33" s="88"/>
+      <c r="V33" s="88"/>
       <c r="W33" s="13"/>
       <c r="X33" s="49"/>
     </row>
@@ -9853,7 +9861,7 @@
       <c r="B34" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="C34" s="87" t="s">
+      <c r="C34" s="68" t="s">
         <v>336</v>
       </c>
       <c r="D34" s="6"/>
@@ -9894,7 +9902,7 @@
       <c r="B35" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C35" s="86" t="s">
+      <c r="C35" s="67" t="s">
         <v>326</v>
       </c>
       <c r="D35" s="1"/>
@@ -9935,10 +9943,10 @@
       <c r="B36" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C36" s="87" t="s">
+      <c r="C36" s="68" t="s">
         <v>331</v>
       </c>
-      <c r="D36" s="103" t="s">
+      <c r="D36" s="84" t="s">
         <v>337</v>
       </c>
       <c r="E36" s="2"/>
@@ -9972,10 +9980,10 @@
       <c r="B37" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C37" s="86" t="s">
+      <c r="C37" s="67" t="s">
         <v>336</v>
       </c>
-      <c r="D37" s="101" t="s">
+      <c r="D37" s="82" t="s">
         <v>330</v>
       </c>
       <c r="E37" s="2"/>
@@ -10001,21 +10009,21 @@
       <c r="X37" s="49"/>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="R38" s="71" t="s">
+      <c r="R38" s="95" t="s">
         <v>290</v>
       </c>
-      <c r="S38" s="72"/>
-      <c r="T38" s="72"/>
-      <c r="U38" s="72"/>
+      <c r="S38" s="96"/>
+      <c r="T38" s="96"/>
+      <c r="U38" s="96"/>
       <c r="V38" s="13"/>
       <c r="W38" s="13"/>
       <c r="X38" s="49"/>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="R39" s="71"/>
-      <c r="S39" s="72"/>
-      <c r="T39" s="72"/>
-      <c r="U39" s="72"/>
+      <c r="R39" s="95"/>
+      <c r="S39" s="96"/>
+      <c r="T39" s="96"/>
+      <c r="U39" s="96"/>
       <c r="V39" s="13"/>
       <c r="W39" s="13"/>
       <c r="X39" s="49"/>
@@ -10039,23 +10047,23 @@
       <c r="S41" s="51" t="s">
         <v>281</v>
       </c>
-      <c r="T41" s="76"/>
-      <c r="U41" s="76"/>
+      <c r="T41" s="89"/>
+      <c r="U41" s="89"/>
       <c r="V41" s="13"/>
       <c r="W41" s="13"/>
       <c r="X41" s="49"/>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A42" s="75" t="s">
+      <c r="A42" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="75"/>
+      <c r="B42" s="87"/>
       <c r="C42" s="64"/>
       <c r="D42" s="64"/>
-      <c r="E42" s="84" t="s">
+      <c r="E42" s="104" t="s">
         <v>136</v>
       </c>
-      <c r="F42" s="85"/>
+      <c r="F42" s="103"/>
       <c r="G42" s="64"/>
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
@@ -10140,7 +10148,7 @@
       <c r="B44" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="C44" s="91"/>
+      <c r="C44" s="72"/>
       <c r="D44" s="31"/>
       <c r="E44" s="31" t="s">
         <v>255</v>
@@ -10184,7 +10192,7 @@
       <c r="B45" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C45" s="86" t="s">
+      <c r="C45" s="67" t="s">
         <v>338</v>
       </c>
       <c r="D45" s="1"/>
@@ -10235,10 +10243,10 @@
       <c r="B46" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C46" s="86" t="s">
+      <c r="C46" s="67" t="s">
         <v>339</v>
       </c>
-      <c r="D46" s="101" t="s">
+      <c r="D46" s="82" t="s">
         <v>340</v>
       </c>
       <c r="E46" s="2"/>
@@ -10282,7 +10290,7 @@
       <c r="B47" s="30" t="s">
         <v>238</v>
       </c>
-      <c r="C47" s="92"/>
+      <c r="C47" s="73"/>
       <c r="D47" s="30"/>
       <c r="E47" s="30" t="s">
         <v>256</v>
@@ -10326,7 +10334,7 @@
       <c r="B48" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="87" t="s">
+      <c r="C48" s="68" t="s">
         <v>326</v>
       </c>
       <c r="D48" s="6"/>
@@ -10362,7 +10370,7 @@
       <c r="B49" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C49" s="86" t="s">
+      <c r="C49" s="67" t="s">
         <v>326</v>
       </c>
       <c r="D49" s="1"/>
@@ -10397,7 +10405,7 @@
       <c r="B50" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C50" s="86" t="s">
+      <c r="C50" s="67" t="s">
         <v>326</v>
       </c>
       <c r="D50" s="1"/>
@@ -10419,8 +10427,8 @@
       <c r="S50" s="51" t="s">
         <v>281</v>
       </c>
-      <c r="T50" s="76"/>
-      <c r="U50" s="76"/>
+      <c r="T50" s="89"/>
+      <c r="U50" s="89"/>
       <c r="V50" s="13"/>
       <c r="W50" s="13"/>
       <c r="X50" s="49"/>
@@ -10432,7 +10440,7 @@
       <c r="B51" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C51" s="86" t="s">
+      <c r="C51" s="67" t="s">
         <v>326</v>
       </c>
       <c r="D51" s="1"/>
@@ -10465,7 +10473,7 @@
       <c r="B52" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C52" s="86" t="s">
+      <c r="C52" s="67" t="s">
         <v>326</v>
       </c>
       <c r="D52" s="1"/>
@@ -10508,10 +10516,10 @@
       <c r="B53" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="C53" s="87" t="s">
+      <c r="C53" s="68" t="s">
         <v>341</v>
       </c>
-      <c r="D53" s="103" t="s">
+      <c r="D53" s="84" t="s">
         <v>342</v>
       </c>
       <c r="E53" s="2"/>
@@ -10553,7 +10561,7 @@
       <c r="B54" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C54" s="87" t="s">
+      <c r="C54" s="68" t="s">
         <v>326</v>
       </c>
       <c r="D54" s="6"/>
@@ -10596,7 +10604,7 @@
       <c r="B55" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C55" s="86" t="s">
+      <c r="C55" s="67" t="s">
         <v>343</v>
       </c>
       <c r="D55" s="1"/>
@@ -10637,7 +10645,7 @@
       <c r="B56" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C56" s="86" t="s">
+      <c r="C56" s="67" t="s">
         <v>326</v>
       </c>
       <c r="D56" s="1"/>
@@ -10680,7 +10688,7 @@
       <c r="B57" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C57" s="86" t="s">
+      <c r="C57" s="67" t="s">
         <v>343</v>
       </c>
       <c r="D57" s="1"/>
@@ -10721,7 +10729,7 @@
       <c r="X57" s="49"/>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A58" s="100" t="s">
+      <c r="A58" s="81" t="s">
         <v>345</v>
       </c>
       <c r="R58" s="50"/>
@@ -10743,7 +10751,7 @@
       <c r="X58" s="49"/>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A59" s="98" t="s">
+      <c r="A59" s="79" t="s">
         <v>352</v>
       </c>
       <c r="R59" s="50"/>
@@ -10765,7 +10773,7 @@
       <c r="X59" s="49"/>
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A60" s="99" t="s">
+      <c r="A60" s="80" t="s">
         <v>344</v>
       </c>
       <c r="R60" s="50"/>
@@ -10777,8 +10785,8 @@
       <c r="X60" s="49"/>
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A61" s="99" t="s">
-        <v>379</v>
+      <c r="A61" s="80" t="s">
+        <v>378</v>
       </c>
       <c r="R61" s="61"/>
       <c r="S61" s="62"/>
@@ -10789,16 +10797,16 @@
       <c r="X61" s="63"/>
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A62" s="75" t="s">
+      <c r="A62" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B62" s="75"/>
+      <c r="B62" s="87"/>
       <c r="C62" s="64"/>
       <c r="D62" s="64"/>
-      <c r="E62" s="84" t="s">
+      <c r="E62" s="104" t="s">
         <v>249</v>
       </c>
-      <c r="F62" s="85"/>
+      <c r="F62" s="103"/>
       <c r="G62" s="64"/>
       <c r="H62" s="9"/>
       <c r="I62" s="9"/>
@@ -10866,7 +10874,7 @@
       <c r="B64" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="C64" s="91"/>
+      <c r="C64" s="72"/>
       <c r="D64" s="31"/>
       <c r="E64" s="31" t="s">
         <v>255</v>
@@ -10895,7 +10903,7 @@
       <c r="B65" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C65" s="86"/>
+      <c r="C65" s="67"/>
       <c r="D65" s="1"/>
       <c r="E65" s="17" t="s">
         <v>190</v>
@@ -10929,8 +10937,8 @@
       <c r="B66" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C66" s="86"/>
-      <c r="D66" s="101" t="s">
+      <c r="C66" s="67"/>
+      <c r="D66" s="82" t="s">
         <v>346</v>
       </c>
       <c r="E66" s="2"/>
@@ -10959,7 +10967,7 @@
       <c r="B67" s="30" t="s">
         <v>238</v>
       </c>
-      <c r="C67" s="92"/>
+      <c r="C67" s="73"/>
       <c r="D67" s="30"/>
       <c r="E67" s="30" t="s">
         <v>256</v>
@@ -10988,7 +10996,7 @@
       <c r="B68" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C68" s="87"/>
+      <c r="C68" s="68"/>
       <c r="D68" s="6"/>
       <c r="E68" s="6"/>
       <c r="F68" s="6" t="s">
@@ -11015,8 +11023,10 @@
       <c r="B69" s="30" t="s">
         <v>224</v>
       </c>
-      <c r="C69" s="92"/>
-      <c r="D69" s="30"/>
+      <c r="C69" s="73"/>
+      <c r="D69" s="82" t="s">
+        <v>380</v>
+      </c>
       <c r="E69" s="30" t="s">
         <v>226</v>
       </c>
@@ -11044,7 +11054,7 @@
       <c r="B70" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C70" s="86"/>
+      <c r="C70" s="67"/>
       <c r="D70" s="1"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2" t="s">
@@ -11068,8 +11078,8 @@
       <c r="B71" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C71" s="86"/>
-      <c r="D71" s="101" t="s">
+      <c r="C71" s="67"/>
+      <c r="D71" s="82" t="s">
         <v>373</v>
       </c>
       <c r="E71" s="2"/>
@@ -11094,7 +11104,7 @@
       <c r="B72" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C72" s="86"/>
+      <c r="C72" s="67"/>
       <c r="D72" s="1"/>
       <c r="E72" s="2"/>
       <c r="F72" s="2" t="s">
@@ -11119,8 +11129,8 @@
       <c r="B73" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C73" s="86"/>
-      <c r="D73" s="101" t="s">
+      <c r="C73" s="67"/>
+      <c r="D73" s="82" t="s">
         <v>374</v>
       </c>
       <c r="E73" s="6"/>
@@ -11145,8 +11155,8 @@
       <c r="B74" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C74" s="86"/>
-      <c r="D74" s="101" t="s">
+      <c r="C74" s="67"/>
+      <c r="D74" s="82" t="s">
         <v>375</v>
       </c>
       <c r="E74" s="2"/>
@@ -11177,8 +11187,9 @@
       <c r="B75" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C75" s="86"/>
-      <c r="D75" s="1"/>
+      <c r="C75" s="82" t="s">
+        <v>380</v>
+      </c>
       <c r="E75" s="2"/>
       <c r="F75" s="2" t="s">
         <v>178</v>
@@ -11205,8 +11216,9 @@
       <c r="B76" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C76" s="86"/>
-      <c r="D76" s="1"/>
+      <c r="C76" s="82" t="s">
+        <v>380</v>
+      </c>
       <c r="E76" s="2"/>
       <c r="F76" s="2" t="s">
         <v>178</v>
@@ -11233,7 +11245,7 @@
       <c r="B77" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="C77" s="87"/>
+      <c r="C77" s="68"/>
       <c r="D77" s="6"/>
       <c r="E77" s="2"/>
       <c r="F77" s="2" t="s">
@@ -11262,9 +11274,9 @@
       <c r="B78" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C78" s="87"/>
-      <c r="D78" s="103" t="s">
-        <v>376</v>
+      <c r="C78" s="68"/>
+      <c r="D78" s="84" t="s">
+        <v>382</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78" s="2" t="s">
@@ -11293,7 +11305,7 @@
       <c r="B79" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C79" s="86"/>
+      <c r="C79" s="67"/>
       <c r="D79" s="1"/>
       <c r="E79" s="2"/>
       <c r="F79" s="2" t="s">
@@ -11317,7 +11329,7 @@
       <c r="B80" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C80" s="86"/>
+      <c r="C80" s="67"/>
       <c r="D80" s="1"/>
       <c r="E80" s="2"/>
       <c r="F80" s="2" t="s">
@@ -11343,7 +11355,7 @@
       <c r="B81" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C81" s="86"/>
+      <c r="C81" s="67"/>
       <c r="D81" s="1"/>
       <c r="E81" s="17" t="s">
         <v>195</v>
@@ -11367,7 +11379,7 @@
       <c r="W81" s="13"/>
     </row>
     <row r="82" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A82" s="100" t="s">
+      <c r="A82" s="81" t="s">
         <v>345</v>
       </c>
       <c r="R82" s="13"/>
@@ -11377,7 +11389,7 @@
       <c r="V82" s="13"/>
     </row>
     <row r="83" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A83" s="98" t="s">
+      <c r="A83" s="79" t="s">
         <v>352</v>
       </c>
       <c r="R83" s="13"/>
@@ -11387,7 +11399,7 @@
       <c r="V83" s="13"/>
     </row>
     <row r="84" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A84" s="99" t="s">
+      <c r="A84" s="80" t="s">
         <v>344</v>
       </c>
       <c r="S84" s="13"/>
@@ -11396,8 +11408,8 @@
       <c r="V84" s="13"/>
     </row>
     <row r="85" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A85" s="99" t="s">
-        <v>379</v>
+      <c r="A85" s="80" t="s">
+        <v>378</v>
       </c>
       <c r="S85" s="13"/>
       <c r="T85" s="13"/>
@@ -11405,16 +11417,16 @@
       <c r="V85" s="13"/>
     </row>
     <row r="86" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="75" t="s">
+      <c r="A86" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B86" s="75"/>
+      <c r="B86" s="87"/>
       <c r="C86" s="64"/>
       <c r="D86" s="64"/>
-      <c r="E86" s="84" t="s">
+      <c r="E86" s="104" t="s">
         <v>246</v>
       </c>
-      <c r="F86" s="85"/>
+      <c r="F86" s="103"/>
       <c r="G86" s="64"/>
       <c r="H86" s="9"/>
       <c r="I86" s="9"/>
@@ -11433,7 +11445,7 @@
       <c r="B87" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C87" s="93"/>
+      <c r="C87" s="74"/>
       <c r="D87" s="14"/>
       <c r="E87" s="14" t="s">
         <v>3</v>
@@ -11473,7 +11485,7 @@
       <c r="B88" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="C88" s="93"/>
+      <c r="C88" s="74"/>
       <c r="D88" s="14"/>
       <c r="E88" s="14" t="s">
         <v>264</v>
@@ -11502,7 +11514,7 @@
       <c r="B89" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C89" s="87"/>
+      <c r="C89" s="68"/>
       <c r="D89" s="6"/>
       <c r="E89" s="6"/>
       <c r="F89" s="6" t="s">
@@ -11531,7 +11543,7 @@
       <c r="B90" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C90" s="87"/>
+      <c r="C90" s="68"/>
       <c r="D90" s="6"/>
       <c r="E90" s="6"/>
       <c r="F90" s="6" t="s">
@@ -11555,7 +11567,7 @@
       <c r="B91" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="C91" s="87"/>
+      <c r="C91" s="68"/>
       <c r="D91" s="6"/>
       <c r="E91" s="2"/>
       <c r="F91" s="2" t="s">
@@ -11580,7 +11592,7 @@
       <c r="B92" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="C92" s="87"/>
+      <c r="C92" s="68"/>
       <c r="D92" s="6"/>
       <c r="E92" s="2"/>
       <c r="F92" s="2" t="s">
@@ -11602,7 +11614,7 @@
       <c r="B93" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="C93" s="87"/>
+      <c r="C93" s="68"/>
       <c r="D93" s="6"/>
       <c r="E93" s="2"/>
       <c r="F93" s="2" t="s">
@@ -11626,7 +11638,7 @@
       <c r="B94" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="C94" s="87"/>
+      <c r="C94" s="68"/>
       <c r="D94" s="6"/>
       <c r="E94" s="2"/>
       <c r="F94" s="2" t="s">
@@ -11654,7 +11666,7 @@
       <c r="B95" s="31" t="s">
         <v>223</v>
       </c>
-      <c r="C95" s="91"/>
+      <c r="C95" s="72"/>
       <c r="D95" s="31"/>
       <c r="E95" s="31"/>
       <c r="F95" s="30" t="s">
@@ -11681,7 +11693,7 @@
       <c r="B96" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="C96" s="87"/>
+      <c r="C96" s="68"/>
       <c r="D96" s="6"/>
       <c r="E96" s="2"/>
       <c r="F96" s="6" t="s">
@@ -11699,21 +11711,21 @@
       <c r="N96" s="2"/>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A97" s="100" t="s">
+      <c r="A97" s="81" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A100" s="75" t="s">
+      <c r="A100" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B100" s="75"/>
+      <c r="B100" s="87"/>
       <c r="C100" s="64"/>
       <c r="D100" s="64"/>
-      <c r="E100" s="84" t="s">
+      <c r="E100" s="104" t="s">
         <v>247</v>
       </c>
-      <c r="F100" s="85"/>
+      <c r="F100" s="103"/>
       <c r="G100" s="64"/>
       <c r="H100" s="9"/>
       <c r="I100" s="9"/>
@@ -11770,7 +11782,7 @@
       <c r="B102" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="C102" s="93"/>
+      <c r="C102" s="74"/>
       <c r="D102" s="14"/>
       <c r="E102" s="14" t="s">
         <v>265</v>
@@ -11799,7 +11811,7 @@
       <c r="B103" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C103" s="86"/>
+      <c r="C103" s="67"/>
       <c r="D103" s="1"/>
       <c r="E103" s="6"/>
       <c r="F103" s="6" t="s">
@@ -11830,7 +11842,7 @@
       <c r="B104" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C104" s="86"/>
+      <c r="C104" s="67"/>
       <c r="D104" s="1"/>
       <c r="E104" s="6" t="s">
         <v>226</v>
@@ -11856,7 +11868,7 @@
       <c r="B105" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C105" s="86"/>
+      <c r="C105" s="67"/>
       <c r="D105" s="1"/>
       <c r="E105" s="2"/>
       <c r="F105" s="2" t="s">
@@ -11880,9 +11892,9 @@
       <c r="B106" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C106" s="86"/>
-      <c r="D106" s="101" t="s">
-        <v>377</v>
+      <c r="C106" s="67"/>
+      <c r="D106" s="82" t="s">
+        <v>376</v>
       </c>
       <c r="E106" s="2"/>
       <c r="F106" s="2" t="s">
@@ -11906,7 +11918,7 @@
       <c r="B107" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="C107" s="87"/>
+      <c r="C107" s="68"/>
       <c r="D107" s="6"/>
       <c r="E107" s="2"/>
       <c r="F107" s="2" t="s">
@@ -11928,7 +11940,7 @@
       <c r="B108" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="C108" s="87"/>
+      <c r="C108" s="68"/>
       <c r="D108" s="6"/>
       <c r="E108" s="2"/>
       <c r="F108" s="2" t="s">
@@ -11952,7 +11964,7 @@
       <c r="B109" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C109" s="86"/>
+      <c r="C109" s="67"/>
       <c r="D109" s="1"/>
       <c r="E109" s="2" t="s">
         <v>227</v>
@@ -11978,7 +11990,7 @@
       <c r="B110" s="31" t="s">
         <v>223</v>
       </c>
-      <c r="C110" s="91"/>
+      <c r="C110" s="72"/>
       <c r="D110" s="31"/>
       <c r="E110" s="31"/>
       <c r="F110" s="30" t="s">
@@ -12002,7 +12014,7 @@
       <c r="B111" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="C111" s="87"/>
+      <c r="C111" s="68"/>
       <c r="D111" s="6"/>
       <c r="E111" s="2"/>
       <c r="F111" s="6" t="s">
@@ -12020,26 +12032,26 @@
       <c r="N111" s="2"/>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A112" s="100" t="s">
+      <c r="A112" s="81" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="113" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A113" s="100" t="s">
+      <c r="A113" s="81" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="115" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A115" s="75" t="s">
+      <c r="A115" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B115" s="75"/>
+      <c r="B115" s="87"/>
       <c r="C115" s="64"/>
       <c r="D115" s="64"/>
-      <c r="E115" s="82" t="s">
+      <c r="E115" s="102" t="s">
         <v>349</v>
       </c>
-      <c r="F115" s="85"/>
+      <c r="F115" s="103"/>
       <c r="G115" s="64"/>
       <c r="H115" s="9"/>
       <c r="I115" s="9"/>
@@ -12098,8 +12110,10 @@
       <c r="B117" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="C117" s="91"/>
-      <c r="D117" s="31"/>
+      <c r="C117" s="72"/>
+      <c r="D117" s="31" t="s">
+        <v>381</v>
+      </c>
       <c r="E117" s="31" t="s">
         <v>255</v>
       </c>
@@ -12131,7 +12145,7 @@
       <c r="B118" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C118" s="86"/>
+      <c r="C118" s="67"/>
       <c r="D118" s="1"/>
       <c r="E118" s="2" t="s">
         <v>198</v>
@@ -12166,7 +12180,7 @@
       <c r="B119" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C119" s="86"/>
+      <c r="C119" s="67"/>
       <c r="D119" s="1"/>
       <c r="E119" s="22" t="s">
         <v>220</v>
@@ -12199,7 +12213,7 @@
       <c r="B120" s="33" t="s">
         <v>222</v>
       </c>
-      <c r="C120" s="94"/>
+      <c r="C120" s="75"/>
       <c r="D120" s="33"/>
       <c r="E120" s="33" t="s">
         <v>265</v>
@@ -12235,7 +12249,7 @@
       <c r="B121" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C121" s="87"/>
+      <c r="C121" s="68"/>
       <c r="D121" s="6"/>
       <c r="E121" s="6"/>
       <c r="F121" s="6" t="s">
@@ -12263,7 +12277,7 @@
       <c r="B122" s="30" t="s">
         <v>224</v>
       </c>
-      <c r="C122" s="92"/>
+      <c r="C122" s="73"/>
       <c r="D122" s="30"/>
       <c r="E122" s="30" t="s">
         <v>226</v>
@@ -12294,7 +12308,7 @@
       <c r="B123" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C123" s="87"/>
+      <c r="C123" s="68"/>
       <c r="D123" s="6"/>
       <c r="E123" s="2"/>
       <c r="F123" s="2" t="s">
@@ -12320,8 +12334,8 @@
       <c r="B124" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="C124" s="87"/>
-      <c r="D124" s="103" t="s">
+      <c r="C124" s="68"/>
+      <c r="D124" s="84" t="s">
         <v>354</v>
       </c>
       <c r="E124" s="2" t="s">
@@ -12350,8 +12364,8 @@
       <c r="B125" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C125" s="95"/>
-      <c r="D125" s="101" t="s">
+      <c r="C125" s="76"/>
+      <c r="D125" s="82" t="s">
         <v>350</v>
       </c>
       <c r="E125" s="2"/>
@@ -12376,7 +12390,7 @@
       <c r="B126" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C126" s="86"/>
+      <c r="C126" s="67"/>
       <c r="D126" s="1"/>
       <c r="E126" s="2"/>
       <c r="F126" s="2" t="s">
@@ -12401,7 +12415,7 @@
       <c r="B127" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C127" s="86"/>
+      <c r="C127" s="67"/>
       <c r="D127" s="1"/>
       <c r="E127" s="17" t="s">
         <v>216</v>
@@ -12428,7 +12442,7 @@
       <c r="V127" s="19"/>
     </row>
     <row r="128" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A128" s="98" t="s">
+      <c r="A128" s="79" t="s">
         <v>352</v>
       </c>
       <c r="O128" s="1"/>
@@ -12438,94 +12452,94 @@
       <c r="V128" s="19"/>
     </row>
     <row r="129" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A129" s="99" t="s">
+      <c r="A129" s="80" t="s">
         <v>344</v>
       </c>
       <c r="O129" s="1"/>
     </row>
     <row r="130" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A130" s="101" t="s">
+      <c r="A130" s="82" t="s">
         <v>121</v>
       </c>
       <c r="O130" s="1"/>
     </row>
     <row r="131" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A131" s="101" t="s">
+      <c r="A131" s="82" t="s">
         <v>21</v>
       </c>
       <c r="O131" s="1"/>
     </row>
     <row r="132" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A132" s="101" t="s">
+      <c r="A132" s="82" t="s">
         <v>124</v>
       </c>
       <c r="O132" s="1"/>
     </row>
     <row r="133" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A133" s="101" t="s">
+      <c r="A133" s="82" t="s">
         <v>125</v>
       </c>
       <c r="O133" s="1"/>
     </row>
     <row r="134" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A134" s="101" t="s">
+      <c r="A134" s="82" t="s">
         <v>126</v>
       </c>
       <c r="O134" s="1"/>
     </row>
     <row r="135" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A135" s="101" t="s">
+      <c r="A135" s="82" t="s">
         <v>127</v>
       </c>
       <c r="O135" s="1"/>
     </row>
     <row r="136" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A136" s="101" t="s">
+      <c r="A136" s="82" t="s">
         <v>129</v>
       </c>
       <c r="O136" s="1"/>
     </row>
     <row r="137" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A137" s="101" t="s">
+      <c r="A137" s="82" t="s">
         <v>130</v>
       </c>
       <c r="O137" s="1"/>
     </row>
     <row r="138" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A138" s="101" t="s">
+      <c r="A138" s="82" t="s">
         <v>131</v>
       </c>
       <c r="O138" s="1"/>
     </row>
     <row r="139" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A139" s="101" t="s">
-        <v>378</v>
+      <c r="A139" s="82" t="s">
+        <v>377</v>
       </c>
       <c r="O139" s="1"/>
     </row>
     <row r="140" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A140" s="103" t="s">
+      <c r="A140" s="84" t="s">
         <v>133</v>
       </c>
       <c r="O140" s="1"/>
     </row>
     <row r="141" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A141" s="98" t="s">
-        <v>380</v>
+      <c r="A141" s="79" t="s">
+        <v>379</v>
       </c>
       <c r="O141" s="6"/>
     </row>
     <row r="142" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A142" s="75" t="s">
+      <c r="A142" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B142" s="75"/>
+      <c r="B142" s="87"/>
       <c r="C142" s="64"/>
       <c r="D142" s="64"/>
-      <c r="E142" s="84" t="s">
+      <c r="E142" s="104" t="s">
         <v>85</v>
       </c>
-      <c r="F142" s="85"/>
+      <c r="F142" s="103"/>
       <c r="G142" s="64"/>
       <c r="H142" s="9"/>
       <c r="I142" s="9"/>
@@ -12575,7 +12589,7 @@
       <c r="N143" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="O143" s="98"/>
+      <c r="O143" s="79"/>
     </row>
     <row r="144" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A144" s="7" t="s">
@@ -12584,8 +12598,8 @@
       <c r="B144" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C144" s="86"/>
-      <c r="D144" s="101" t="s">
+      <c r="C144" s="67"/>
+      <c r="D144" s="82" t="s">
         <v>356</v>
       </c>
       <c r="E144" s="17" t="s">
@@ -12606,7 +12620,7 @@
       <c r="N144" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="O144" s="99"/>
+      <c r="O144" s="80"/>
     </row>
     <row r="145" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A145" s="31" t="s">
@@ -12615,8 +12629,8 @@
       <c r="B145" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="C145" s="91"/>
-      <c r="D145" s="105" t="s">
+      <c r="C145" s="72"/>
+      <c r="D145" s="86" t="s">
         <v>360</v>
       </c>
       <c r="E145" s="31" t="s">
@@ -12643,7 +12657,7 @@
       <c r="B146" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C146" s="86"/>
+      <c r="C146" s="67"/>
       <c r="D146" s="1"/>
       <c r="E146" s="17" t="s">
         <v>190</v>
@@ -12671,7 +12685,7 @@
       <c r="B147" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C147" s="86"/>
+      <c r="C147" s="67"/>
       <c r="D147" s="1"/>
       <c r="E147" s="2"/>
       <c r="F147" s="2" t="s">
@@ -12695,7 +12709,7 @@
       <c r="B148" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C148" s="86"/>
+      <c r="C148" s="67"/>
       <c r="D148" s="1"/>
       <c r="E148" s="2"/>
       <c r="F148" s="2" t="s">
@@ -12719,8 +12733,8 @@
       <c r="B149" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C149" s="86"/>
-      <c r="D149" s="104" t="s">
+      <c r="C149" s="67"/>
+      <c r="D149" s="85" t="s">
         <v>358</v>
       </c>
       <c r="E149" s="2" t="s">
@@ -12748,7 +12762,7 @@
       <c r="B150" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C150" s="102" t="s">
+      <c r="C150" s="83" t="s">
         <v>355</v>
       </c>
       <c r="D150" s="1"/>
@@ -12775,7 +12789,7 @@
       <c r="B151" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C151" s="86"/>
+      <c r="C151" s="67"/>
       <c r="D151" s="1"/>
       <c r="E151" s="2"/>
       <c r="F151" s="22" t="s">
@@ -12792,34 +12806,34 @@
       <c r="Q151" s="13"/>
     </row>
     <row r="152" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A152" s="100" t="s">
+      <c r="A152" s="81" t="s">
         <v>361</v>
       </c>
       <c r="Q152" s="13"/>
     </row>
     <row r="153" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A153" s="100" t="s">
+      <c r="A153" s="81" t="s">
         <v>359</v>
       </c>
       <c r="Q153" s="13"/>
     </row>
     <row r="154" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A154" s="98" t="s">
+      <c r="A154" s="79" t="s">
         <v>363</v>
       </c>
       <c r="R154" s="13"/>
     </row>
     <row r="155" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A155" s="75" t="s">
+      <c r="A155" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B155" s="75"/>
+      <c r="B155" s="87"/>
       <c r="C155" s="64"/>
       <c r="D155" s="64"/>
-      <c r="E155" s="84" t="s">
+      <c r="E155" s="104" t="s">
         <v>166</v>
       </c>
-      <c r="F155" s="85"/>
+      <c r="F155" s="103"/>
       <c r="G155" s="64"/>
       <c r="H155" s="9"/>
       <c r="I155" s="9"/>
@@ -12878,7 +12892,7 @@
       <c r="B157" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C157" s="86"/>
+      <c r="C157" s="67"/>
       <c r="D157" s="1"/>
       <c r="E157" s="6"/>
       <c r="F157" s="6" t="s">
@@ -12903,7 +12917,7 @@
       <c r="B158" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C158" s="86"/>
+      <c r="C158" s="67"/>
       <c r="D158" s="1"/>
       <c r="E158" s="2"/>
       <c r="F158" s="2" t="s">
@@ -12928,7 +12942,7 @@
       <c r="B159" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="C159" s="95"/>
+      <c r="C159" s="76"/>
       <c r="D159" s="5"/>
       <c r="E159" s="2"/>
       <c r="F159" s="2" t="s">
@@ -12952,7 +12966,7 @@
       <c r="B160" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C160" s="86"/>
+      <c r="C160" s="67"/>
       <c r="D160" s="1"/>
       <c r="E160" s="2"/>
       <c r="F160" s="2" t="s">
@@ -12976,7 +12990,7 @@
       <c r="B161" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C161" s="87"/>
+      <c r="C161" s="68"/>
       <c r="D161" s="6"/>
       <c r="E161" s="2"/>
       <c r="F161" s="2" t="s">
@@ -13000,8 +13014,8 @@
       <c r="B162" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C162" s="86"/>
-      <c r="D162" s="101" t="s">
+      <c r="C162" s="67"/>
+      <c r="D162" s="82" t="s">
         <v>364</v>
       </c>
       <c r="E162" s="2"/>
@@ -13020,26 +13034,26 @@
       <c r="N162" s="2"/>
     </row>
     <row r="163" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A163" s="100" t="s">
+      <c r="A163" s="81" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="164" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A164" s="100" t="s">
+      <c r="A164" s="81" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="166" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A166" s="75" t="s">
+      <c r="A166" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B166" s="75"/>
+      <c r="B166" s="87"/>
       <c r="C166" s="64"/>
       <c r="D166" s="64"/>
-      <c r="E166" s="84" t="s">
+      <c r="E166" s="104" t="s">
         <v>237</v>
       </c>
-      <c r="F166" s="85"/>
+      <c r="F166" s="103"/>
       <c r="G166" s="64"/>
       <c r="H166" s="9"/>
       <c r="I166" s="9"/>
@@ -13096,7 +13110,7 @@
       <c r="B168" s="30" t="s">
         <v>238</v>
       </c>
-      <c r="C168" s="92"/>
+      <c r="C168" s="73"/>
       <c r="D168" s="30"/>
       <c r="E168" s="30" t="s">
         <v>256</v>
@@ -13124,7 +13138,7 @@
       <c r="B169" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="C169" s="86"/>
+      <c r="C169" s="67"/>
       <c r="D169" s="1"/>
       <c r="E169" s="2"/>
       <c r="F169" s="6" t="s">
@@ -13142,11 +13156,11 @@
       <c r="N169" s="2"/>
     </row>
     <row r="170" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="99" t="s">
+      <c r="A170" s="80" t="s">
         <v>367</v>
       </c>
       <c r="B170" s="27"/>
-      <c r="C170" s="96"/>
+      <c r="C170" s="77"/>
       <c r="D170" s="27"/>
       <c r="R170"/>
       <c r="S170"/>
@@ -13158,7 +13172,7 @@
     <row r="171" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="26"/>
       <c r="B171" s="26"/>
-      <c r="C171" s="97"/>
+      <c r="C171" s="78"/>
       <c r="D171" s="26"/>
       <c r="G171" s="28"/>
       <c r="R171"/>
@@ -13171,7 +13185,7 @@
     <row r="172" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="29"/>
       <c r="B172" s="29"/>
-      <c r="C172" s="89"/>
+      <c r="C172" s="70"/>
       <c r="D172" s="29"/>
       <c r="G172" s="28"/>
       <c r="R172"/>
@@ -13182,16 +13196,16 @@
       <c r="W172"/>
     </row>
     <row r="173" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A173" s="75" t="s">
+      <c r="A173" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B173" s="75"/>
+      <c r="B173" s="87"/>
       <c r="C173" s="64"/>
       <c r="D173" s="64"/>
-      <c r="E173" s="106" t="s">
+      <c r="E173" s="105" t="s">
         <v>368</v>
       </c>
-      <c r="F173" s="85"/>
+      <c r="F173" s="103"/>
       <c r="G173" s="64"/>
       <c r="H173" s="9"/>
       <c r="I173" s="9"/>
@@ -13250,7 +13264,7 @@
       <c r="B175" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="C175" s="86"/>
+      <c r="C175" s="67"/>
       <c r="D175" s="1"/>
       <c r="E175" s="6" t="s">
         <v>293</v>
@@ -13278,8 +13292,8 @@
       <c r="B176" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C176" s="86"/>
-      <c r="D176" s="101" t="s">
+      <c r="C176" s="67"/>
+      <c r="D176" s="82" t="s">
         <v>369</v>
       </c>
       <c r="E176" s="2" t="s">
@@ -13301,13 +13315,13 @@
       <c r="R176" s="13"/>
     </row>
     <row r="177" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A177" s="99" t="s">
+      <c r="A177" s="80" t="s">
         <v>370</v>
       </c>
       <c r="R177" s="13"/>
     </row>
     <row r="178" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A178" s="99" t="s">
+      <c r="A178" s="80" t="s">
         <v>371</v>
       </c>
       <c r="S178" s="13"/>
@@ -13316,7 +13330,7 @@
       <c r="V178" s="13"/>
     </row>
     <row r="179" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A179" s="99" t="s">
+      <c r="A179" s="80" t="s">
         <v>372</v>
       </c>
       <c r="S179" s="13"/>
@@ -13332,6 +13346,26 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="R13:U15"/>
+    <mergeCell ref="U19:V19"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="E100:F100"/>
+    <mergeCell ref="U26:V26"/>
+    <mergeCell ref="U33:V33"/>
+    <mergeCell ref="R38:U39"/>
+    <mergeCell ref="T41:U41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="T50:U50"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="E86:F86"/>
     <mergeCell ref="E115:F115"/>
     <mergeCell ref="A166:B166"/>
     <mergeCell ref="E166:F166"/>
@@ -13342,26 +13376,6 @@
     <mergeCell ref="A115:B115"/>
     <mergeCell ref="A142:B142"/>
     <mergeCell ref="A155:B155"/>
-    <mergeCell ref="T50:U50"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="E86:F86"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="E100:F100"/>
-    <mergeCell ref="U26:V26"/>
-    <mergeCell ref="U33:V33"/>
-    <mergeCell ref="R38:U39"/>
-    <mergeCell ref="T41:U41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="R13:U15"/>
-    <mergeCell ref="U19:V19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="E20:F20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>